<commit_message>
Correção pra ac 05
</commit_message>
<xml_diff>
--- a/12- Lista de Características (Descrição de cada caracteristica).xlsx
+++ b/12- Lista de Características (Descrição de cada caracteristica).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alisson\Desktop\Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\alisson jitador 2.o\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4CB1E1-819F-4988-A135-E3A41E27369E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E98BCEEC-D915-42C6-AA27-C0DBC296A7D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -365,9 +365,6 @@
     <t xml:space="preserve"> (Descrição de cada característica)</t>
   </si>
   <si>
-    <t xml:space="preserve">12. Lista de Características </t>
-  </si>
-  <si>
     <t>Cadastrar Cliente</t>
   </si>
   <si>
@@ -384,6 +381,9 @@
   </si>
   <si>
     <t>O sistema deverá registrar informações sobre o controle de serviços encaminhados, informando para qual parceiro a ordem de serviço foi encaminhada e o status do serviço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lista de Características </t>
   </si>
 </sst>
 </file>
@@ -535,12 +535,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -575,6 +569,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -859,14 +859,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="53.42578125" customWidth="1"/>
@@ -878,11 +878,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="3" t="s">
         <v>111</v>
       </c>
@@ -894,681 +894,681 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="18" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="2:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="16"/>
-      <c r="C5" s="6">
+      <c r="B5" s="14"/>
+      <c r="C5" s="4">
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="6">
+      <c r="B6" s="14"/>
+      <c r="C6" s="4">
         <v>3</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>101</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
-      <c r="C7" s="6">
+      <c r="B7" s="14"/>
+      <c r="C7" s="4">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>102</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="6">
+      <c r="B8" s="14"/>
+      <c r="C8" s="4">
         <v>5</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
-      <c r="C9" s="6">
+      <c r="B9" s="14"/>
+      <c r="C9" s="4">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>56</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
-      <c r="C10" s="6">
+      <c r="B10" s="14"/>
+      <c r="C10" s="4">
         <v>7</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
-      <c r="C11" s="6">
+      <c r="B11" s="14"/>
+      <c r="C11" s="4">
         <v>8</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="6">
+      <c r="B12" s="15"/>
+      <c r="C12" s="4">
         <v>9</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>10</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="57" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="6">
+      <c r="B14" s="14"/>
+      <c r="C14" s="4">
         <v>11</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="6">
+      <c r="B15" s="15"/>
+      <c r="C15" s="4">
         <v>12</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <v>13</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
-      <c r="C17" s="6">
+      <c r="B17" s="14"/>
+      <c r="C17" s="4">
         <v>14</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="6">
+      <c r="B18" s="14"/>
+      <c r="C18" s="4">
         <v>15</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="6">
+      <c r="B19" s="15"/>
+      <c r="C19" s="4">
         <v>16</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="4">
         <v>17</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
-      <c r="C21" s="6">
+      <c r="B21" s="14"/>
+      <c r="C21" s="4">
         <v>18</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="16"/>
-      <c r="C22" s="6">
+      <c r="B22" s="14"/>
+      <c r="C22" s="4">
         <v>19</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="14"/>
+      <c r="C23" s="4">
+        <v>20</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="16"/>
-      <c r="C23" s="6">
+      <c r="E23" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+      <c r="C24" s="4">
+        <v>21</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="4">
+        <v>22</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="57" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+      <c r="C26" s="4">
+        <v>23</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="14"/>
+      <c r="C27" s="4">
+        <v>24</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="15"/>
+      <c r="C28" s="4">
+        <v>25</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="4">
+        <v>26</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="14"/>
+      <c r="C30" s="4">
+        <v>27</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
+      <c r="C31" s="4">
+        <v>28</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="15"/>
+      <c r="C32" s="4">
+        <v>29</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="4">
+        <v>30</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="57" x14ac:dyDescent="0.25">
+      <c r="B34" s="14"/>
+      <c r="C34" s="4">
+        <v>31</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="14"/>
+      <c r="C35" s="4">
+        <v>32</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="15"/>
+      <c r="C36" s="4">
+        <v>33</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="4">
+        <v>34</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="14"/>
+      <c r="C38" s="4">
+        <v>35</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="14"/>
+      <c r="C39" s="4">
+        <v>36</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="15"/>
+      <c r="C40" s="4">
+        <v>37</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="4">
+        <v>38</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
+      <c r="C42" s="4">
+        <v>39</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
-      <c r="C24" s="6">
+      <c r="E42" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="14"/>
+      <c r="C43" s="4">
+        <v>40</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="E43" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="14"/>
+      <c r="C44" s="4">
+        <v>41</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="14"/>
+      <c r="C45" s="4">
+        <v>42</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B46" s="14"/>
+      <c r="C46" s="4">
+        <v>43</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="14"/>
+      <c r="C47" s="4">
+        <v>44</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="14"/>
+      <c r="C48" s="4">
+        <v>45</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B49" s="14"/>
+      <c r="C49" s="4">
+        <v>46</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="14"/>
+      <c r="C50" s="4">
+        <v>47</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="14"/>
+      <c r="C51" s="4">
+        <v>48</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B52" s="14"/>
+      <c r="C52" s="4">
         <v>49</v>
       </c>
-      <c r="C25" s="6">
-        <v>22</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="57" x14ac:dyDescent="0.25">
-      <c r="B26" s="16"/>
-      <c r="C26" s="6">
-        <v>23</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="16"/>
-      <c r="C27" s="6">
-        <v>24</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
-      <c r="C28" s="6">
-        <v>25</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="6">
-        <v>26</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="16"/>
-      <c r="C30" s="6">
-        <v>27</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="16"/>
-      <c r="C31" s="6">
-        <v>28</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="17"/>
-      <c r="C32" s="6">
-        <v>29</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="6">
-        <v>30</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="57" x14ac:dyDescent="0.25">
-      <c r="B34" s="16"/>
-      <c r="C34" s="6">
-        <v>31</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B35" s="16"/>
-      <c r="C35" s="6">
+      <c r="D52" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="14"/>
+      <c r="C53" s="4">
+        <v>50</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="156.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="14"/>
+      <c r="C54" s="4">
+        <v>51</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="17"/>
-      <c r="C36" s="6">
-        <v>33</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="6">
-        <v>34</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="16"/>
-      <c r="C38" s="6">
-        <v>35</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="16"/>
-      <c r="C39" s="6">
-        <v>36</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="17"/>
-      <c r="C40" s="6">
-        <v>37</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="6">
-        <v>38</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="7" t="s">
+      <c r="E54" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="15"/>
+      <c r="C55" s="4">
+        <v>52</v>
+      </c>
+      <c r="D55" s="11" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="16"/>
-      <c r="C42" s="6">
-        <v>39</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="16"/>
-      <c r="C43" s="6">
-        <v>40</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="16"/>
-      <c r="C44" s="6">
-        <v>41</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="16"/>
-      <c r="C45" s="6">
-        <v>42</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B46" s="16"/>
-      <c r="C46" s="6">
-        <v>43</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16"/>
-      <c r="C47" s="6">
-        <v>44</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="16"/>
-      <c r="C48" s="6">
-        <v>45</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="16"/>
-      <c r="C49" s="6">
-        <v>46</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="16"/>
-      <c r="C50" s="6">
-        <v>47</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="16"/>
-      <c r="C51" s="6">
-        <v>48</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B52" s="16"/>
-      <c r="C52" s="6">
-        <v>49</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="16"/>
-      <c r="C53" s="6">
-        <v>50</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="156.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="16"/>
-      <c r="C54" s="6">
-        <v>51</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="57.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="17"/>
-      <c r="C55" s="6">
-        <v>52</v>
-      </c>
-      <c r="D55" s="13" t="s">
+      <c r="E55" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B4:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="B41:B55"/>
     <mergeCell ref="B20:B24"/>
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>

</xml_diff>